<commit_message>
Deploying to gh-pages from  @ b837028956e9348ece1d6d9fda8f721dff557311 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/4.c.1.xlsx
+++ b/en/downloads/data-excel/4.c.1.xlsx
@@ -28,15 +28,6 @@
     <t>(в процентах)</t>
   </si>
   <si>
-    <t>4.c.1.1  Доля дипломированных учителей в образовательных учереждениях</t>
-  </si>
-  <si>
-    <t>4.с.1.1 Билим берүү мекемелерде диплом берилгем мугалимдердин үлүшү</t>
-  </si>
-  <si>
-    <t>4.c.1.1 Proportion of certified teachers in educational institutions</t>
-  </si>
-  <si>
     <t>а) мектепке чейинки билим берүү уюмдарында</t>
   </si>
   <si>
@@ -68,6 +59,15 @@
   </si>
   <si>
     <t>Items</t>
+  </si>
+  <si>
+    <t>4.с.1 Билим берүү мекемелерде диплом берилгем мугалимдердин үлүшү</t>
+  </si>
+  <si>
+    <t>4.c.1 Доля дипломированных учителей в образовательных учереждениях</t>
+  </si>
+  <si>
+    <t>4.c.1 Proportion of certified teachers in educational institutions</t>
   </si>
 </sst>
 </file>
@@ -500,7 +500,7 @@
   <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.25"/>
@@ -511,24 +511,24 @@
   <sheetData>
     <row r="1" spans="1:13" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -548,13 +548,13 @@
     </row>
     <row r="4" spans="1:13" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D4" s="7">
         <v>2010</v>
@@ -589,13 +589,13 @@
     </row>
     <row r="5" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D5" s="4">
         <v>87.9</v>
@@ -630,13 +630,13 @@
     </row>
     <row r="6" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D6" s="4">
         <v>93.6</v>
@@ -671,13 +671,13 @@
     </row>
     <row r="7" spans="1:13" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>2</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D7" s="5">
         <v>92.9</v>

</xml_diff>